<commit_message>
[FIX] Fixed a typo and deleted the lock file
</commit_message>
<xml_diff>
--- a/table import/avvistamenti.xlsx
+++ b/table import/avvistamenti.xlsx
@@ -167,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -201,11 +201,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -263,24 +258,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,27 +348,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="16.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="48.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="48.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,7 +418,7 @@
       <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -452,7 +443,7 @@
       <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -477,7 +468,7 @@
       <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -502,7 +493,7 @@
       <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -527,7 +518,7 @@
       <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -552,7 +543,7 @@
       <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -577,7 +568,7 @@
       <c r="G8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -602,7 +593,7 @@
       <c r="G9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -627,7 +618,7 @@
       <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -652,7 +643,7 @@
       <c r="G11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="I11" s="3" t="s">
@@ -677,7 +668,7 @@
       <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I12" s="3" t="s">

</xml_diff>

<commit_message>
[FIX] Fixed some issues with the insert queries
</commit_message>
<xml_diff>
--- a/table import/avvistamenti.xlsx
+++ b/table import/avvistamenti.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">W7UXUWRWBN</t>
   </si>
   <si>
-    <t xml:space="preserve">Utilizzando lo zoom per vedere meglio l’esmplare, il team si è accorto che i filamenti seghettati della medusa si muovono, probabilmente significando che trasportano le sostanze nutritive al resto del corpo.</t>
+    <t xml:space="preserve">Utilizzando lo zoom per vedere meglio l’esemplare, il team si è accorto che i filamenti seghettati della medusa si muovono, probabilmente significando che trasportano le sostanze nutritive al resto del corpo.</t>
   </si>
   <si>
     <t xml:space="preserve">A69M3QUS9A</t>
@@ -348,25 +348,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="16.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="48.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.34"/>
   </cols>

</xml_diff>

<commit_message>
[MOD] Removed image from the database and changed the app accordingly
</commit_message>
<xml_diff>
--- a/table import/avvistamenti.xlsx
+++ b/table import/avvistamenti.xlsx
@@ -20,20 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Numero</t>
-  </si>
-  <si>
     <t xml:space="preserve">Profondità</t>
   </si>
   <si>
-    <t xml:space="preserve">Foto</t>
-  </si>
-  <si>
     <t xml:space="preserve">Note</t>
   </si>
   <si>
@@ -55,13 +49,13 @@
     <t xml:space="preserve">null</t>
   </si>
   <si>
-    <t xml:space="preserve">L’esemplare sembra “fluttuare” in posizione verticale, con il mantello rivolto verso il basso.</t>
+    <t xml:space="preserve">L’esemplare sembra fluttuare in posizione verticale, con il mantello rivolto verso il basso.</t>
   </si>
   <si>
     <t xml:space="preserve">UDPDW13YB8</t>
   </si>
   <si>
-    <t xml:space="preserve">Alaska</t>
+    <t xml:space="preserve">VJ4EIJACWK</t>
   </si>
   <si>
     <t xml:space="preserve">7876I2RYN3</t>
@@ -79,6 +73,9 @@
     <t xml:space="preserve">364FIFD9JR</t>
   </si>
   <si>
+    <t xml:space="preserve">FKCHELYUK3</t>
+  </si>
+  <si>
     <t xml:space="preserve">W7UXUWRWBN</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
     <t xml:space="preserve">P4FPZBSA8O</t>
   </si>
   <si>
+    <t xml:space="preserve">SSEY2O52BP</t>
+  </si>
+  <si>
     <t xml:space="preserve">FRG2FXY0E5</t>
   </si>
   <si>
@@ -127,37 +127,10 @@
     <t xml:space="preserve">JTXMQ1M1JV</t>
   </si>
   <si>
-    <t xml:space="preserve">L’esemplare sembra muoversi all’interno della sua “casa” di muco che utilizza per filtrare i nutrimenti. La massa di muco è completamente trasparente e sembra catturare diverse particelle fluttuanti presenti nell’acqua.</t>
+    <t xml:space="preserve">L’esemplare sembra muoversi all’interno della sua casa di muco che utilizza per filtrare i nutrimenti. La massa di muco è completamente trasparente e sembra catturare diverse particelle fluttuanti presenti nell’acqua.</t>
   </si>
   <si>
     <t xml:space="preserve">6567LBSV3P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7IN6FK4UQR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UGRE37ZRL0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G6Q129AYN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORQ1R3YC9P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4MBE4FILM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDKSS4BO5U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OV2X22VENQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F81BHDU40K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VCAZB5TLIG</t>
   </si>
 </sst>
 </file>
@@ -352,23 +325,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="48.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="48.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,406 +364,342 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="71.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="57.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="57.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="3" t="n">
+        <v>700</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="n">
-        <v>700</v>
-      </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E9" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="n">
+      <c r="B10" s="3" t="n">
         <v>900</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="71.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>40</v>
-      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>41</v>
-      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>42</v>
-      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>43</v>
-      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>44</v>
-      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>45</v>
-      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -800,10 +707,8 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -811,10 +716,8 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -822,10 +725,8 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -833,10 +734,8 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -844,10 +743,8 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -855,10 +752,8 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -866,10 +761,8 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -877,10 +770,8 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -888,8 +779,6 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>